<commit_message>
descw-1253 step3 - get basic model and report output
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_43_rpt_PF_RecoveryForecast.xlsx
+++ b/backend/reports/xlsx/Tab_43_rpt_PF_RecoveryForecast.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496916F9-3500-554E-AF29-D6EE385AE044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475AAFE-242F-EB40-B9C8-ABA653D9D8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
-  <si>
-    <t>TOTAL:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
@@ -71,45 +68,6 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>{$r.project_number}</t>
-  </si>
-  <si>
-    <t>{$r1.project_number}</t>
-  </si>
-  <si>
-    <t>{$r.project_name}</t>
-  </si>
-  <si>
-    <t>{$r.q1}</t>
-  </si>
-  <si>
-    <t>{$r.q2}</t>
-  </si>
-  <si>
-    <t>{$r.q3}</t>
-  </si>
-  <si>
-    <t>{$r.q4}</t>
-  </si>
-  <si>
-    <t>{$r.q_total}</t>
-  </si>
-  <si>
-    <t>{$t.q1_total}</t>
-  </si>
-  <si>
-    <t>{$t.grand_total}</t>
-  </si>
-  <si>
-    <t>{$t.q3_total}</t>
-  </si>
-  <si>
-    <t>{$t.q4_total}</t>
-  </si>
-  <si>
-    <t>{$t.q2_total}</t>
-  </si>
-  <si>
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
@@ -117,12 +75,6 @@
   </si>
   <si>
     <t>Total Forecast</t>
-  </si>
-  <si>
-    <t>{$r.project_status}</t>
-  </si>
-  <si>
-    <t>{$r.recoverable_status}</t>
   </si>
   <si>
     <t>Project
@@ -304,17 +256,17 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,7 +649,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="A3" sqref="A3:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -708,135 +660,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="33" thickBot="1">
       <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>10</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="6"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -844,12 +754,12 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -858,9 +768,10 @@
     <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="5" scale="89" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
-    <oddFooter>&amp;Lrpt_PF_NetRecoverySummaryByQuarter&amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>
+    <oddFooter>&amp;LTab_43_rpt_PF_RecoveryForecast
+&amp;C&amp;P of &amp;N&amp;R{$date}</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
descw-1253 add carbone templating language to .xls
* update the .xlsx file with specific fields from model
* add minor formatting
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_43_rpt_PF_RecoveryForecast.xlsx
+++ b/backend/reports/xlsx/Tab_43_rpt_PF_RecoveryForecast.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4475AAFE-242F-EB40-B9C8-ABA653D9D8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B303DC5A-8FA0-9A42-BDA4-5B4263D37CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
   <si>
     <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
   </si>
   <si>
     <t>{#date=d.date}</t>
@@ -83,6 +80,57 @@
   <si>
     <t>Recoverable
 Status</t>
+  </si>
+  <si>
+    <t>{#t=d.totals[i]}</t>
+  </si>
+  <si>
+    <t>Totals:</t>
+  </si>
+  <si>
+    <t>{$t.sum_q1}</t>
+  </si>
+  <si>
+    <t>{$t.total_forecast}</t>
+  </si>
+  <si>
+    <t>{$t.sum_q2}</t>
+  </si>
+  <si>
+    <t>{$t.sum_q3}</t>
+  </si>
+  <si>
+    <t>{$t.sum_q4}</t>
+  </si>
+  <si>
+    <t>{$r.project_number}</t>
+  </si>
+  <si>
+    <t>{$r.project_name}</t>
+  </si>
+  <si>
+    <t>{$r.project_status}</t>
+  </si>
+  <si>
+    <t>{$r.recoverable}</t>
+  </si>
+  <si>
+    <t>{$r.q1_amount}</t>
+  </si>
+  <si>
+    <t>{$r.q2_amount}</t>
+  </si>
+  <si>
+    <t>{$r.q3_amount}</t>
+  </si>
+  <si>
+    <t>{$r.q4_amount}</t>
+  </si>
+  <si>
+    <t>{$r.total_forecast}</t>
+  </si>
+  <si>
+    <t>{$r1.project_number}</t>
   </si>
 </sst>
 </file>
@@ -92,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +176,11 @@
       <color theme="1"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8.5"/>
+      <name val="BCSans-Regular"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -224,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -266,6 +319,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -649,7 +705,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I5"/>
+      <selection activeCell="E5" sqref="E5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -663,7 +719,7 @@
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
       <c r="C1" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -674,46 +730,66 @@
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="33" thickBot="1">
       <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>9</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -727,12 +803,24 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
@@ -746,7 +834,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -754,12 +842,12 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>